<commit_message>
Add: Game score. Update: Decoration
</commit_message>
<xml_diff>
--- a/Group Contribution.xlsx
+++ b/Group Contribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiroh\Desktop\2048\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA96C8F-ED45-4812-A17A-23AF1BA7997B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295B5FD9-66C4-48F0-947E-90EF32FAF5F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{894AB7D6-2077-4295-9151-0CE026D3FB07}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,13 +567,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>20</v>
       </c>
       <c r="E4" s="2">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2">
         <v>20</v>
@@ -642,7 +642,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="3">
         <f>SUM(C3:C7) / SUM(C3:F7)*100</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3">
         <f>SUM(D3:D7)/SUM(C3:F7)*100</f>
@@ -650,7 +650,7 @@
       </c>
       <c r="E8" s="3">
         <f>SUM(E3:E7)/SUM(C3:F7)*100</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3">
         <f>SUM(F3:F7)/SUM(C3:F7)*100</f>

</xml_diff>